<commit_message>
Minor updates to case studies.
</commit_message>
<xml_diff>
--- a/input_files/UC_case_study_5bus_network_A.xlsx
+++ b/input_files/UC_case_study_5bus_network_A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bus index" sheetId="5" r:id="rId1"/>
@@ -192,9 +192,6 @@
     <t>Bubble SEN Wind 2014-2045_0910refyr.csv</t>
   </si>
   <si>
-    <t>Bubble NEN Wind 2014-2045_0910refyr.csv</t>
-  </si>
-  <si>
     <t>CAN Solar PV.csv</t>
   </si>
   <si>
@@ -208,6 +205,9 @@
   </si>
   <si>
     <t>Node 2 includes busses 1 &amp; 2 (node numbering chosen to match bus numbers for simplicity)</t>
+  </si>
+  <si>
+    <t>Bubble HUN Wind 2014-2045_0910refyr.csv</t>
   </si>
 </sst>
 </file>
@@ -217,12 +217,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -249,8 +250,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +270,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE9D9"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -288,7 +303,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="663">
+  <cellStyleXfs count="681">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -952,8 +967,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -980,8 +1013,11 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="663">
+  <cellStyles count="681">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1313,6 +1349,15 @@
     <cellStyle name="Followed Hyperlink" xfId="658" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="660" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="662" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="664" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="666" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="668" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="670" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="672" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="674" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="676" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="678" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="680" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1644,6 +1689,15 @@
     <cellStyle name="Hyperlink" xfId="657" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="659" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="661" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="663" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="665" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="667" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="669" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="671" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="673" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="675" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="677" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="679" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1975,8 +2029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2020,8 +2074,8 @@
       <c r="C2" s="5">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>56</v>
+      <c r="D2" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>41</v>
@@ -2041,7 +2095,7 @@
         <v>55</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2058,7 +2112,7 @@
         <v>42</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2072,10 +2126,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2111,7 +2165,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2153,14 +2207,14 @@
         <v>2</v>
       </c>
       <c r="C2" s="9">
-        <f t="shared" ref="C2:C8" si="0">(PI()/6)/(E2/100)*D2</f>
-        <v>1.4959965017094252E-2</v>
+        <f>(PI()/12)/(E2/100)*D2</f>
+        <v>1.3089969389957471E-2</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="F2" s="5">
         <v>0</v>
@@ -2174,14 +2228,14 @@
         <v>3</v>
       </c>
       <c r="C3" s="9">
-        <f t="shared" si="0"/>
-        <v>1.4959965017094252E-2</v>
+        <f>(PI()/12)/(E3/100)*D3</f>
+        <v>1.3089969389957471E-2</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" s="5">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="F3" s="5">
         <v>0</v>
@@ -2195,14 +2249,14 @@
         <v>3</v>
       </c>
       <c r="C4" s="9">
-        <f t="shared" si="0"/>
-        <v>1.8699956271367814E-2</v>
+        <f t="shared" ref="C4:C8" si="0">(PI()/6)/(E4/100)*D4</f>
+        <v>1.9392547244381438E-2</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>2800</v>
+        <v>2700</v>
       </c>
       <c r="F4" s="5">
         <v>0</v>
@@ -2216,14 +2270,14 @@
         <v>4</v>
       </c>
       <c r="C5" s="9">
-        <f t="shared" si="0"/>
-        <v>2.0943951023931952E-2</v>
+        <f>(PI()/3)/(E5/100)*D5</f>
+        <v>5.8177641733144311E-2</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="5">
-        <v>2500</v>
+        <v>1800</v>
       </c>
       <c r="F5" s="5">
         <v>0</v>
@@ -2238,13 +2292,13 @@
       </c>
       <c r="C6" s="9">
         <f t="shared" si="0"/>
-        <v>1.0471975511965976E-2</v>
+        <v>1.0908307824964559E-2</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="E6" s="5">
-        <v>5000</v>
+        <v>4800</v>
       </c>
       <c r="F6" s="5">
         <v>0</v>
@@ -2280,13 +2334,13 @@
       </c>
       <c r="C8" s="9">
         <f t="shared" si="0"/>
-        <v>1.1635528346628862E-2</v>
+        <v>1.1382582078223888E-2</v>
       </c>
       <c r="D8" s="5">
         <v>1</v>
       </c>
       <c r="E8" s="5">
-        <v>4500</v>
+        <v>4600</v>
       </c>
       <c r="F8" s="5">
         <v>0</v>
@@ -2307,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2359,7 +2413,7 @@
         <v>50</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6">

</xml_diff>

<commit_message>
Added demand traces at each node to results struct.
</commit_message>
<xml_diff>
--- a/input_files/UC_case_study_5bus_network_A.xlsx
+++ b/input_files/UC_case_study_5bus_network_A.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Bus index" sheetId="5" r:id="rId1"/>
@@ -223,7 +223,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2029,7 +2028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2165,7 +2164,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2482,8 +2481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>